<commit_message>
sn: update tas form
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Senegal/2023/jul 2023/sn_lf_pretas_1_sites_202307.xlsx
+++ b/LF/PreTAS/Senegal/2023/jul 2023/sn_lf_pretas_1_sites_202307.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\PreTAS\Senegal\2023\jul 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23583F8-9DB3-4F09-9395-ABDF25A8D28D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC56605-9BBB-4FB0-BBB7-1482D9A1D1D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -330,12 +330,6 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Juillet 2022) 1. Pre-TAS FL - Formulaire Site V1</t>
-  </si>
-  <si>
-    <t>sn_lf_pretas_1_sites_202207_v1</t>
-  </si>
-  <si>
     <t>French</t>
   </si>
   <si>
@@ -376,6 +370,12 @@
   </si>
   <si>
     <t>Site de contrôle</t>
+  </si>
+  <si>
+    <t>sn_lf_pretas_1_sites_202307</t>
+  </si>
+  <si>
+    <t>(Juillet 2023) 1. Pre-TAS FL - Formulaire Site</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -398,7 +398,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -406,21 +406,21 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -534,11 +534,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -621,7 +621,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -644,6 +644,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -929,7 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1172,14 +1175,14 @@
         <v>70</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" s="36"/>
       <c r="E7" s="37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="18"/>
@@ -1192,7 +1195,7 @@
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
       <c r="P7" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:16" s="14" customFormat="1" ht="15.75" customHeight="1">
@@ -1560,13 +1563,13 @@
         <v>86</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>93</v>
@@ -1606,13 +1609,13 @@
         <v>87</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="10" t="s">
@@ -1624,17 +1627,17 @@
         <v>87</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="5" customFormat="1">
@@ -1642,17 +1645,17 @@
         <v>87</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1">
@@ -1660,13 +1663,13 @@
         <v>87</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="10" t="s">
@@ -1695,7 +1698,7 @@
       </c>
       <c r="E15" s="13"/>
       <c r="G15" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="5" customFormat="1">
@@ -1713,7 +1716,7 @@
       </c>
       <c r="E16" s="13"/>
       <c r="G16" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="5" customFormat="1">
@@ -1731,7 +1734,7 @@
       </c>
       <c r="E17" s="13"/>
       <c r="G17" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1">
@@ -1749,7 +1752,7 @@
       </c>
       <c r="E18" s="13"/>
       <c r="G18" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1765,8 +1768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1787,14 +1790,14 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" t="s">
         <v>98</v>
-      </c>
-      <c r="B2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1825,31 +1828,31 @@
   <sheetData>
     <row r="1" spans="1:12" ht="46.5">
       <c r="A1" s="28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B1" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="33" t="s">
+      <c r="H1" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="L1" s="28" t="s">
         <v>102</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="18.75">
@@ -1860,7 +1863,7 @@
         <v>93</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" s="1">
         <v>101</v>
@@ -1872,13 +1875,13 @@
         <v>93</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K2" s="29" t="s">
         <v>93</v>
       </c>
       <c r="L2" s="30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="18.75">
@@ -1889,7 +1892,7 @@
         <v>93</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" s="1">
         <v>102</v>
@@ -1902,10 +1905,10 @@
         <v>93</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="18.75">
@@ -1913,10 +1916,10 @@
         <v>93</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" s="1">
         <v>103</v>
@@ -1925,10 +1928,10 @@
       <c r="H4" s="32"/>
       <c r="I4" s="32"/>
       <c r="K4" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L4" s="31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="18.75">
@@ -1936,10 +1939,10 @@
         <v>93</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D5" s="1">
         <v>104</v>
@@ -1951,7 +1954,7 @@
         <v>93</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:12">

</xml_diff>